<commit_message>
- gegevens van DDFK toegevoegd
</commit_message>
<xml_diff>
--- a/data/HODOR_DATASOURCE.xlsx
+++ b/data/HODOR_DATASOURCE.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduard\ownCloud\ontwikkelen\github.com\GegevensVergelijker.metwijzigingen\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="233">
   <si>
     <t>NAME</t>
   </si>
@@ -4353,18 +4348,321 @@
   <si>
     <t>Server=sqlservername;Initial Catalog=databasename;Integrated Security=SSPI;</t>
   </si>
+  <si>
+    <t>DDFK_DDS_GVG_ADRACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- Actieve adressen in DDS tbv GISVG
+-- Let op: in te richten paramters voor:
+-- gemeentekode en
+-- applicatenr van GISVG in DDS
+select  adr.adrnr,
+  ind.sleutelsrv,
+  ind.sleutelcli,
+  ind.dating,
+  adr.datend,
+  ind.applicatienr,
+  ind.onderwerpcode,
+  adr.dating,
+  adr.datend,
+  adr.sttnam,
+  dds_tekensetconversie.teletex2unicode(adr.sttnam_d) AS Straatnaam,
+  --adr.gemkde,
+  --adr.obrnam,
+  --adr.sttnam_u,
+  --adr.sttnam_d,
+  adr.huinum,
+  adr.huitvg,
+  adr.huilet,
+  adr.pkdnum,
+  --adr.wplnam,
+  dds_tekensetconversie.teletex2unicode(adr.wplnam) AS Woonplaats,
+  --adr.obrnam_d,
+  adr.identna,
+  adr.vbonr
+from dds_adr_opslag adr join dds_indicatie ind on adr.adrnr = ind.sleutelsrv
+where adr.datend is null
+and  adr.identna is not null
+-- Let op: aanpassen gemeentekode
+-- Deze aanpassing ook aanbrengen in selectie voor GISVG
+and  adr.gemkde = 58 -- Alleen adressen 'eigen' gemeente
+and  adr.datend is null
+and  ind.onderwerpcode = 'ADR'
+-- Let op: aanpassen applicatienr naar die voor GISVG in DDS
+-- opzoeken juiste applicatienr: 
+-- select * from dds_applicatie order by applicatiecode;
+and  ind.applicatienr = 13 
+order by wplnam, sttnam, huinum, huitvg, huilet
+</t>
+  </si>
+  <si>
+    <t>DDFK_GISVG_ADR_ALLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- GISVG Alle adressen voor 'eigen' gemeente
+select adr.ident,
+  adr.postkode,
+  ( nvl(adr.straat || ' ', '') || 
+   nvl(to_char(trunc(adr.huisnr)) || ' ', '') || 
+   nvl(adr.huislt || ' ', '') || 
+   nvl(adr.huistv,'') || 
+   nvl(adr.huisad || ' ', '')
+  ) c3,
+  adr.huisnr, 
+  adr.huislt, 
+  adr.huistv, 
+  adr.huisad, 
+  adr.lokatie, 
+  adr.soort, 
+  adr.strtkd_str, 
+  adr.wplkd_str, 
+  adr.gemkd_gem, 
+  adr.lndkd_lnd, 
+  adr.ident_ptt, 
+  adr.straat, 
+  adr.woonplaats, 
+  adr.landnaam, 
+  adr.datum_einde, 
+  adr.ind_authentiek, 
+  adr.ind_onderzoek, 
+  adr.dds_blokkeren,
+  adr.gemkd_gem
+from pbspbt adr
+where (adr.lndkd_lnd = 6030 or adr.lndkd_lnd is null)
+and  adr.gemkd_gem = '1891' -- Alleen adressen 'eigen' gemeente
+order by c3 asc
+</t>
+  </si>
+  <si>
+    <t>DDFK_GISVG_ADRSUBJACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-- GISVG - subjecten met adressen actief
+-- Let op: aanpassen gemeentekode
+select distinct
+  pers.reg_nr,
+  pers.ident_pbt,
+  adr.straat,
+  adr.huisnr,
+  adr.huislt,
+  adr.huistv,
+  adr.woonplaats,
+  adr.postkode,
+  adr.ident,
+  pers.gebnaam,
+  pers.geb_datum,
+  pers.aanspreeknaam_bl_zv,
+  adrend.soort_adres,
+  ( nvl(adr.straat || ' ', '') || 
+   nvl(to_char(trunc(adr.huisnr)) || ' ', '') || 
+   nvl(adr.huislt || ' ', '') || 
+   nvl(adr.huistv,'') || 
+   nvl(adr.huisad || ' ', '')
+  ) c4,
+  -- Universeel SQL equivalent voor niet-Oracle databases:
+  /*((((case  when not T3.STRAAT is null then (T3.STRAAT || ' ') else '' end  || 
+   case  when not T3.HUISNR is null then (TO_CHAR(TRUNC(T3.HUISNR ) ) || ' ') else '' end ) || 
+   case  when not T3.HUISLT is null then (T3.HUISLT || ' ') else '' end ) || 
+   DECODE(T3.HUISTV,NULL,'' , T3.HUISTV)) || 
+   case  when not T3.HUISAD is null then (T3.HUISAD || ' ') else '' end 
+  ) c4, */
+  nvl(adr.huislt||' ', '') hslet,
+  adrend.datend, 
+  pers.soort_persoon, 
+  pers.sofi_nr, 
+  pers.sofi_nr_aanv, 
+  pers.kvk_nummer, 
+  pers.handelsregnr, 
+  adr.ident
+from pbspsn pers left outer join pbspsa adrend on pers.reg_nr=AdrEnd.reg_nr_psn
+  left outer join pbspbt adr on pers.ident_pbt=adr.ident
+where AdrEnd.datend is null
+--and adr.huislt is null
+--and adr.ident = '141138'
+-- Let op: aanpassen gemeentekode
+and  adr.gemkd_gem = '1891' -- Alleen adressen 'eigen' gemeente
+order by reg_nr asc
+</t>
+  </si>
+  <si>
+    <t>DDFK_OB_DDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/*
+OB:
+ Gegevensmagazijn - actuele personen
+ Contact: 
+ A-nummer 
+ BSN 
+ Voorvoegsel* 
+ Geslachtsnaam* 
+ Geboortedatum 
+ Geboorteplaats 
+ Geslacht* 
+ Postcode* 
+ Straatnaam 
+ Huisnummer* 
+ Huisletter* 
+ Huisnummertoevoeging*
+*/
+SELECT
+  prso.admnum,
+  prso.sofnum,
+  prso.gesvvg,
+  dds_tekensetconversie.teletex2unicode(prso.gesnam_d) AS geslachtsnaam,
+  prso.gebdat,
+  dds_tekensetconversie.teletex2unicode(COALESCE(dds_gemeente.gemeente, prso.gebgmn)) AS geboortegemeente,
+  prso.gebgmn,
+  prso.gesand,
+  --adro.sttnam_d,
+  dds_tekensetconversie.teletex2unicode(adro.obrnam_d) AS openbareruimtenaam,
+  adro.huinum,
+  adro.huilet,
+  adro.huitvg,
+  --adro.huiand,  
+  adro.pkdnum,  
+  --adro.wplnam,
+  dds_tekensetconversie.teletex2unicode(adro.wplnam_bag) AS woonplaats,
+  adro.identobr,
+  adro.identna,
+  adro.identtgo,
+  vboo.identvbo
+FROM
+  DDS_PRS_OPSLAG prso
+INNER JOIN DDS_PRSADR_OPSLAG padr
+  ON prso.PRSNR = padr.PRSNR
+  AND (prso.indgba = 'J' OR prso.indbasispersoon = 'J')
+INNER JOIN DDS_ADR_OPSLAG adro
+  ON padr.ADRNR = adro.ADRNR
+  AND padr.SRTADR = 'I'
+  AND PADR.DATEND is null
+LEFT OUTER JOIN DDS_PREDIKAAT pred
+  ON PRED.PREDIKAAT = PRSO.ADLPRE
+INNER JOIN DDS_VBO_OPSLAG vboo
+  ON adro.ADRNR = vboo.ADRNR
+LEFT OUTER JOIN DDS_GEMEENTE dds_gemeente
+ON 
+(
+ -- RARE DDS OOK ALTIJD
+ to_char(dds_gemeente.gemeentecode) LIKE prso.gebgmn 
+ OR 
+ '0' || to_char(dds_gemeente.gemeentecode) LIKE prso.gebgmn 
+ OR
+ '00' || to_char(dds_gemeente.gemeentecode) LIKE prso.gebgmn 
+ OR
+ '000' || to_char(dds_gemeente.gemeentecode) LIKE prso.gebgmn 
+ OR
+ dds_gemeente.gemeente LIKE prso.gebgmn     
+)
+/
+</t>
+  </si>
+  <si>
+    <t>DDFK_R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/*
+R2:
+        GBA - actuele personen
+        Contact: A.Kraak@gemeenteswf.nl
+        A-nummer*      
+        BSN*     
+        Voorvoegsel*   
+        Geslachtsnaam*             
+        Geboortedatum*           
+        Geboorteplaats*            
+        Geslacht*           
+        Postcode*          
+        Straatnaam        
+        Huisnummer*  
+        Huisletter*         
+        Huisnummertoevoeging*           
+        Datum huwelijkssluiting/geregistreerd partnerschap* 
+        Datum ontbinding huwelijkssluiting/geregistreerd partnerschap*
+*/
+/*
+SELECT 
+  GBA_VSELAKTP.administratienummer AS anummer,
+  GBA_VSELAKTP.bsn,
+  GBA_VSELAKTP.voornaam,
+  GBA_VSELAKTP.voorvoegsel,
+  GBA_VSELAKTP.geslachtsnaam,
+  GBA_VSELAKTP.geboortedatum,
+  GBA_VSELAKTP.geboorteplaatsnaam AS geboorteplaats,
+  GBA_VSELAKTP.kode_geslacht AS geslacht,
+  GBA_VSELAKTP.POSTKODE_NUMERIEK || GBA_VSELAKTP.POSTKODE_ALFANUMERIEK AS postcode, 
+  -- GBA_VSELAKTP.straatnaam,
+  GBA_VSELADRS.""NAAM_OPENBARE_RUIMTE"" AS openbareruimtenaam,   
+  GBA_VSELAKTP.huisnummer,
+  GBA_VSELAKTP.huisletter,      
+  GBA_VSELAKTP.toevoeging_huisnummer AS huisnummertoevoeging,
+  GBA_VSELADRS.GEMEENTEDEEL AS WOONPLAATS,
+  GBA_VSELADRS.IDENT_VERBLIJFPLAATS, 
+  GBA_VSELADRS.IDENT_NUMMERAANDUIDING,
+  GBA_VSELHUW.DATUM_HUWELIJK,
+  GBA_VSELHUW.DATUM_HUWELIJKSONTBINDING
+FROM
+  PRODPIV.GBA_VSELAKTP@PPIV
+JOIN PRODPIV.GBA_VSELADRS@PPIV
+  ON GBA_VSELAKTP.SYSTEEMNUMMER_ADRES = GBA_VSELADRS.SYSTEEMNUMMER_ADRES
+JOIN PRODPIV.GBA_VSELHUW@PPIV
+  ON GBA_VSELAKTP.SYSTEEMNUMMER_PERSOON = GBA_VSELHUW.SYSTEEMNUMMER_PERSOON
+--WHERE GBA_VSELAKTP.administratienummer = 9245906875
+*/
+SELECT 
+  GBA_VSELAKTP.administratienummer AS anummer,
+  GBA_VSELAKTP.bsn,
+  GBA_VSELAKTP.voornaam,
+  GBA_VSELAKTP.voorvoegsel,
+  GBA_VSELAKTP.geslachtsnaam,
+  GBA_VSELAKTP.geboortedatum,
+  GBA_VSELAKTP.geboorteplaatsnaam AS geboorteplaats,
+  GBA_VSELAKTP.kode_geslacht AS geslacht,
+  GBA_VSELAKTP.POSTKODE_NUMERIEK || GBA_VSELAKTP.POSTKODE_ALFANUMERIEK AS postcode, 
+  -- GBA_VSELAKTP.straatnaam,
+  GBA_VSELADRS.""NAAM_OPENBARE_RUIMTE"" AS openbareruimtenaam,
+  GBA_VSELADRS.straatnaam,
+  GBA_VSELADRS.straatnaam_TLX,
+  GBA_VSELADRS.straatnaam_ZD,
+  GBA_VSELAKTP.huisnummer,
+  GBA_VSELAKTP.huisletter,      
+  GBA_VSELAKTP.toevoeging_huisnummer AS huisnummertoevoeging,
+  GBA_VSELADRS.GEMEENTEDEEL AS WOONPLAATS,
+  GBA_VSELADRS.IDENT_VERBLIJFPLAATS, 
+  GBA_VSELADRS.IDENT_NUMMERAANDUIDING,
+  GBA_VSELHUW.DATUM_HUWELIJK,
+  GBA_VSELHUW.DATUM_HUWELIJKSONTBINDING
+FROM
+  PRODPIV.GBA_VSELAKTP
+JOIN PRODPIV.GBA_VSELADRS
+  ON GBA_VSELAKTP.SYSTEEMNUMMER_ADRES = GBA_VSELADRS.SYSTEEMNUMMER_ADRES
+JOIN PRODPIV.GBA_VSELHUW
+  ON GBA_VSELAKTP.SYSTEEMNUMMER_PERSOON = GBA_VSELHUW.SYSTEEMNUMMER_PERSOON
+--WHERE GBA_VSELAKTP.administratienummer = 9245906875
+/
+</t>
+  </si>
+  <si>
+    <t>BUNSCHOTEN_DDS_OVL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4375,7 +4673,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -4383,18 +4681,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4407,8 +4750,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:D110" totalsRowShown="0">
-  <autoFilter ref="A1:D110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:D116" totalsRowShown="0">
+  <autoFilter ref="A1:D116"/>
   <tableColumns count="4">
     <tableColumn id="1" name="NAME"/>
     <tableColumn id="2" name="PROVIDER"/>
@@ -4708,7 +5051,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4719,11 +5062,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="255.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6274,10 +6617,74 @@
         <v>219</v>
       </c>
     </row>
+    <row r="111" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>222</v>
+      </c>
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>224</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>226</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>228</v>
+      </c>
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>230</v>
+      </c>
+      <c r="B115" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>232</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>